<commit_message>
Updateana xls datoteka sa zaduženjima
</commit_message>
<xml_diff>
--- a/DOKUMENTACIJE/Za ispraviti.xlsx
+++ b/DOKUMENTACIJE/Za ispraviti.xlsx
@@ -16,14 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t>Opširnije napisati opis projektnog zadatka</t>
   </si>
   <si>
-    <t>Pisani scenariji: Mogući drugi scenariji moraju navoditi na koju se točku odnose (numeriranje)</t>
-  </si>
-  <si>
     <t>Sekvencijski dijagrami: argumenti, povratne vrijednosti, odgovori (pripaziti na to)</t>
   </si>
   <si>
@@ -33,9 +30,6 @@
     <t>Dijagram kod opisa sustava (ovo pretpostavljam da znate na što se odnosi)</t>
   </si>
   <si>
-    <t>Arhitektura: opis razreda (u jednoj rečenici) i baze podataka; numeracija (ili imena) metodâ/atributâ</t>
-  </si>
-  <si>
     <t>Dijagram objekata: layout? (urediti da tekst ide prije slike)</t>
   </si>
   <si>
@@ -127,6 +121,18 @@
   </si>
   <si>
     <t>Zaključak</t>
+  </si>
+  <si>
+    <t>Arhitektura: opis razreda (u jednoj rečenici) i baze podataka; numeracija/imena metoda/atributa</t>
+  </si>
+  <si>
+    <t>Pisani scenariji: Mogući drugi scenariji - točka na koju se odnose (numeriranje)</t>
+  </si>
+  <si>
+    <t>Antun, Katarina, Zoki</t>
+  </si>
+  <si>
+    <t>Antun</t>
   </si>
 </sst>
 </file>
@@ -162,13 +168,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="5">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -176,16 +186,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -219,56 +219,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -284,11 +234,11 @@
   <autoFilter ref="A1:D9"/>
   <tableColumns count="4">
     <tableColumn id="1" name="#"/>
-    <tableColumn id="2" name="Potrebno ispraviti"/>
+    <tableColumn id="2" name="Potrebno ispraviti" dataDxfId="0"/>
     <tableColumn id="3" name="Tko?"/>
     <tableColumn id="4" name="Status"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -301,7 +251,7 @@
     <tableColumn id="3" name="Tko?"/>
     <tableColumn id="4" name="Status"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -594,255 +544,263 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="89.140625" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="88.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
+      <c r="B3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>3</v>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>4</v>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>5</v>
+      <c r="B7" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>6</v>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>7</v>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
-      </c>
-    </row>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
         <v>17</v>
       </c>
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    </row>
+    <row r="14" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    </row>
+    <row r="17" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>23</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>25</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>27</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>29</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>31</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>33</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D9">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"DA"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"NE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:D22">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"NE"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"DA"</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Excel update + opis dijagrama razreda i dio ovog mog
</commit_message>
<xml_diff>
--- a/DOKUMENTACIJE/Za ispraviti.xlsx
+++ b/DOKUMENTACIJE/Za ispraviti.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
   <si>
     <t>Opširnije napisati opis projektnog zadatka</t>
   </si>
@@ -133,6 +133,18 @@
   </si>
   <si>
     <t>Antun</t>
+  </si>
+  <si>
+    <t>Vukušić, Žagar</t>
+  </si>
+  <si>
+    <t>Katarina, Zoki</t>
+  </si>
+  <si>
+    <t>nadopuniti</t>
+  </si>
+  <si>
+    <t>dodani uvod i opis modela i contollera</t>
   </si>
 </sst>
 </file>
@@ -542,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,7 +568,7 @@
     <col min="4" max="4" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -570,7 +582,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -584,7 +596,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -598,7 +610,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -612,7 +624,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -626,7 +638,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -637,18 +649,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
       <c r="D7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -662,7 +680,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -673,8 +691,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -688,7 +706,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -698,56 +716,89 @@
       <c r="C12" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="B13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
       <c r="B15" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
       <c r="B16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
       <c r="B17" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
       <c r="B18" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -755,28 +806,46 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
       <c r="B20" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>31</v>
       </c>
       <c r="B21" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>33</v>
       </c>
       <c r="B22" t="s">
         <v>34</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel + skica sustava
</commit_message>
<xml_diff>
--- a/DOKUMENTACIJE/Za ispraviti.xlsx
+++ b/DOKUMENTACIJE/Za ispraviti.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
   <si>
     <t>Opširnije napisati opis projektnog zadatka</t>
   </si>
@@ -144,7 +144,7 @@
     <t>nadopuniti</t>
   </si>
   <si>
-    <t>dodani uvod i opis modela i contollera</t>
+    <t>DJELOMIČNO: dodani uvod i opis modela i contollera</t>
   </si>
 </sst>
 </file>
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,8 +645,11 @@
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -805,6 +808,9 @@
       <c r="B19" t="s">
         <v>28</v>
       </c>
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -826,6 +832,9 @@
       </c>
       <c r="B21" t="s">
         <v>32</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
       </c>
       <c r="D21" t="s">
         <v>14</v>

</xml_diff>